<commit_message>
add users through end of fall 2018
</commit_message>
<xml_diff>
--- a/UsersLatLong.xlsx
+++ b/UsersLatLong.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20337"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\MacrosystemsEDDIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E095DEB-79BC-40DA-98D2-E6CBFED1DDD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>School</t>
   </si>
@@ -66,14 +67,52 @@
   </si>
   <si>
     <t>WashState</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Wellesley</t>
+  </si>
+  <si>
+    <t>Maine-Farmington</t>
+  </si>
+  <si>
+    <t>St. Norbert</t>
+  </si>
+  <si>
+    <t>Iowa State</t>
+  </si>
+  <si>
+    <t> -88.066357</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,8 +140,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,153 +431,464 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="E2" s="3">
         <v>-87.628088000000005</v>
       </c>
-      <c r="C2">
+      <c r="F2" s="3">
         <v>41.897150000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-74.084907999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>41.738461000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-84.731444999999994</v>
+      </c>
+      <c r="F4" s="3">
+        <v>39.510517</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3">
+        <v>-80.425218999999998</v>
+      </c>
+      <c r="F5" s="3">
+        <v>37.228957000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-80.425218999999998</v>
+      </c>
+      <c r="F6" s="3">
+        <v>37.228957000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="E7" s="3">
         <v>-69.663505000000001</v>
       </c>
-      <c r="C3">
+      <c r="F7" s="3">
         <v>44.563907</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="E8" s="3">
         <v>-6.4059999999999997</v>
       </c>
-      <c r="C4">
+      <c r="F8" s="3">
         <v>53.997900000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="E9" s="3">
         <v>-73.264730999999998</v>
       </c>
-      <c r="C5">
+      <c r="F9" s="3">
         <v>41.149915999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="E10" s="3">
         <v>-77.073706999999999</v>
       </c>
-      <c r="C6">
+      <c r="F10" s="3">
         <v>38.908588000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="E11" s="3">
         <v>-78.396861999999999</v>
       </c>
-      <c r="C7">
+      <c r="F11" s="3">
         <v>37.297136999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="E12" s="3">
         <v>-84.482761999999994</v>
       </c>
-      <c r="C8">
+      <c r="F12" s="3">
         <v>42.701051999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>-74.084907999999999</v>
-      </c>
-      <c r="C9">
-        <v>41.738461000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-119.263831</v>
+      </c>
+      <c r="F13" s="3">
+        <v>46.330840000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-80.425218999999998</v>
+      </c>
+      <c r="F14" s="3">
+        <v>37.228957000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3">
+        <v>-80.425218999999998</v>
+      </c>
+      <c r="F15" s="3">
+        <v>37.228957000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3">
+        <v>-119.263831</v>
+      </c>
+      <c r="F16" s="3">
+        <v>46.330840000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3">
+        <v>-78.396861999999999</v>
+      </c>
+      <c r="F17" s="3">
+        <v>37.297136999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="4">
+        <v>-71.306139000000002</v>
+      </c>
+      <c r="F18" s="3">
+        <v>42.293396000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-70.148285999999999</v>
+      </c>
+      <c r="F19" s="3">
+        <v>44.667881999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="3">
+        <v>44.444806</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="E21" s="3">
         <v>-84.731444999999994</v>
       </c>
-      <c r="C10">
+      <c r="F21" s="3">
         <v>39.510517</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>-80.425218999999998</v>
-      </c>
-      <c r="C11">
-        <v>37.228957000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>-119.263831</v>
-      </c>
-      <c r="C12">
-        <v>46.330840000000002</v>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3">
+        <v>3</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="3">
+        <v>-93.644856000000004</v>
+      </c>
+      <c r="F22" s="3">
+        <v>42.026124000000003</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F15">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add new users to MacroEDDIE map for G20 poster
</commit_message>
<xml_diff>
--- a/UsersLatLong.xlsx
+++ b/UsersLatLong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\MacrosystemsEDDIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E095DEB-79BC-40DA-98D2-E6CBFED1DDD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3E1672-4B9E-4B04-A15D-DD6D64FF74F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>School</t>
   </si>
@@ -97,6 +97,48 @@
   </si>
   <si>
     <t> -88.066357</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Washington DC</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
   </si>
 </sst>
 </file>
@@ -432,20 +474,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E23" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -459,13 +502,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -478,14 +524,17 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3">
         <v>-87.628088000000005</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>41.897150000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2017</v>
       </c>
@@ -498,14 +547,17 @@
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3">
         <v>-74.084907999999999</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>41.738461000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2017</v>
       </c>
@@ -518,14 +570,17 @@
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3">
         <v>-84.731444999999994</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>39.510517</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2017</v>
       </c>
@@ -538,14 +593,17 @@
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3">
         <v>-80.425218999999998</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>37.228957000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2017</v>
       </c>
@@ -558,14 +616,17 @@
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3">
         <v>-80.425218999999998</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>37.228957000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2018</v>
       </c>
@@ -578,14 +639,17 @@
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3">
         <v>-69.663505000000001</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>44.563907</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2018</v>
       </c>
@@ -598,14 +662,17 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3">
         <v>-6.4059999999999997</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>53.997900000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2018</v>
       </c>
@@ -618,14 +685,17 @@
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="3">
         <v>-73.264730999999998</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>41.149915999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2018</v>
       </c>
@@ -638,14 +708,17 @@
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3">
         <v>-77.073706999999999</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>38.908588000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2018</v>
       </c>
@@ -658,14 +731,17 @@
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="3">
         <v>-78.396861999999999</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>37.297136999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2018</v>
       </c>
@@ -678,14 +754,17 @@
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="3">
         <v>-84.482761999999994</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>42.701051999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2018</v>
       </c>
@@ -698,14 +777,17 @@
       <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="3">
         <v>-119.263831</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>46.330840000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2018</v>
       </c>
@@ -718,14 +800,17 @@
       <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3">
         <v>-80.425218999999998</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>37.228957000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2018</v>
       </c>
@@ -738,14 +823,17 @@
       <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3">
         <v>-80.425218999999998</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>37.228957000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2018</v>
       </c>
@@ -758,14 +846,17 @@
       <c r="D16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="3">
         <v>-119.263831</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>46.330840000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2018</v>
       </c>
@@ -778,14 +869,17 @@
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3">
         <v>-78.396861999999999</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>37.297136999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2018</v>
       </c>
@@ -798,14 +892,17 @@
       <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="4">
         <v>-71.306139000000002</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>42.293396000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2018</v>
       </c>
@@ -818,14 +915,17 @@
       <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="3">
         <v>-70.148285999999999</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>44.667881999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2018</v>
       </c>
@@ -839,13 +939,16 @@
         <v>21</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>44.444806</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2018</v>
       </c>
@@ -858,14 +961,17 @@
       <c r="D21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="3">
         <v>-84.731444999999994</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>39.510517</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2018</v>
       </c>
@@ -878,15 +984,18 @@
       <c r="D22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="3">
         <v>-93.644856000000004</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
         <v>42.026124000000003</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F15">
+  <sortState ref="A2:G15">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove testers who didn't end up testing
</commit_message>
<xml_diff>
--- a/UsersLatLong.xlsx
+++ b/UsersLatLong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\MacrosystemsEDDIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3E1672-4B9E-4B04-A15D-DD6D64FF74F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5AF8AE-EE4F-4252-A64A-47D710992C7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>School</t>
   </si>
@@ -84,21 +84,12 @@
     <t>Spring</t>
   </si>
   <si>
-    <t>Wellesley</t>
-  </si>
-  <si>
     <t>Maine-Farmington</t>
   </si>
   <si>
-    <t>St. Norbert</t>
-  </si>
-  <si>
     <t>Iowa State</t>
   </si>
   <si>
-    <t> -88.066357</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -133,12 +124,6 @@
   </si>
   <si>
     <t>Washington</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
   </si>
 </sst>
 </file>
@@ -182,16 +167,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -474,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E1:E1048576"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -525,7 +507,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3">
         <v>-87.628088000000005</v>
@@ -548,7 +530,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3">
         <v>-74.084907999999999</v>
@@ -571,7 +553,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3">
         <v>-84.731444999999994</v>
@@ -594,7 +576,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3">
         <v>-80.425218999999998</v>
@@ -617,7 +599,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3">
         <v>-80.425218999999998</v>
@@ -640,7 +622,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="3">
         <v>-69.663505000000001</v>
@@ -663,7 +645,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3">
         <v>-6.4059999999999997</v>
@@ -686,7 +668,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F9" s="3">
         <v>-73.264730999999998</v>
@@ -709,7 +691,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3">
         <v>-77.073706999999999</v>
@@ -732,7 +714,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F11" s="3">
         <v>-78.396861999999999</v>
@@ -755,7 +737,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F12" s="3">
         <v>-84.482761999999994</v>
@@ -778,7 +760,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F13" s="3">
         <v>-119.263831</v>
@@ -801,7 +783,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F14" s="3">
         <v>-80.425218999999998</v>
@@ -824,7 +806,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F15" s="3">
         <v>-80.425218999999998</v>
@@ -847,7 +829,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F16" s="3">
         <v>-119.263831</v>
@@ -867,16 +849,16 @@
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="3">
-        <v>-78.396861999999999</v>
+        <v>-70.148285999999999</v>
       </c>
       <c r="G17" s="3">
-        <v>37.297136999999999</v>
+        <v>44.667881999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -890,16 +872,16 @@
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="4">
-        <v>-71.306139000000002</v>
+        <v>24</v>
+      </c>
+      <c r="F18" s="3">
+        <v>-84.731444999999994</v>
       </c>
       <c r="G18" s="3">
-        <v>42.293396000000001</v>
+        <v>39.510517</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -907,90 +889,21 @@
         <v>2018</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="3">
-        <v>-70.148285999999999</v>
+        <v>-93.644856000000004</v>
       </c>
       <c r="G19" s="3">
-        <v>44.667881999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>2018</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="3">
-        <v>44.444806</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>2018</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="3">
-        <v>-84.731444999999994</v>
-      </c>
-      <c r="G21" s="3">
-        <v>39.510517</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>2018</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="3">
-        <v>3</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="3">
-        <v>-93.644856000000004</v>
-      </c>
-      <c r="G22" s="3">
         <v>42.026124000000003</v>
       </c>
     </row>

</xml_diff>